<commit_message>
finish coverage, still lack of run Commandline javac and java automatically
</commit_message>
<xml_diff>
--- a/target/classes/test_report_template.xlsx
+++ b/target/classes/test_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Haivt\gen-test\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4000CE0C-88A2-4279-993B-DACB0CA33982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B409A01-B8EE-4415-BD6D-C3AA0F78CF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8966F471-EB4F-4157-9CE5-3CECFADF3B80}"/>
   </bookViews>
@@ -470,136 +470,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738CFB42-71AF-406C-BD58-16D80CA741AB}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
-    <col min="5" max="14" width="16.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="13" width="16.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="4"/>
+      <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="L8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="M7:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>